<commit_message>
adapt parser properties to new file format, change test files
</commit_message>
<xml_diff>
--- a/backend/src/test/resources/short_valid_file1.xlsx
+++ b/backend/src/test/resources/short_valid_file1.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Soamid\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D102915-86F1-4313-86DE-9BAFD315AC85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
   <si>
     <t>ID</t>
   </si>
@@ -132,6 +132,24 @@
   </si>
   <si>
     <t>Marchewka lab (+10% do lab);Rabat na sianko (darmowa kartkówka);Lekarstwo (odrobienie 2pkt lab);Weterynarz (odrobienie 1 kartkówki);</t>
+  </si>
+  <si>
+    <t>Grupa (prowadzący):</t>
+  </si>
+  <si>
+    <t>Punkty — Grupa (prowadzący):</t>
+  </si>
+  <si>
+    <t>Opinia — Grupa (prowadzący):</t>
+  </si>
+  <si>
+    <t>Zbigniew Kaleta</t>
+  </si>
+  <si>
+    <t>Michał Idzik</t>
+  </si>
+  <si>
+    <t>Bernard Maj</t>
   </si>
 </sst>
 </file>
@@ -141,7 +159,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,12 +168,36 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u val="single"/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FF0563C1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -175,21 +217,141 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0"/>
+  <cellStyleXfs count="21">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0">
+      <alignment/>
+      <protection/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="20">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment/>
+      <protection/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="15" builtinId="5"/>
+    <cellStyle name="Currency" xfId="16" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="17" builtinId="7"/>
+    <cellStyle name="Comma" xfId="18" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="19" builtinId="6"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -497,185 +659,203 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DF951B8-3D4B-4C21-A79D-223F9A53DA59}">
-  <dimension ref="A1:S4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DF951B8-3D4B-4C21-A79D-223F9A53DA59}">
+  <dimension ref="A1:V4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:AF4"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:19">
-      <c r="A1" t="s">
+    <row r="1" spans="1:22" ht="15" customHeight="1">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="T1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
-      <c r="A2">
+    <row r="2" spans="1:20" ht="15" customHeight="1">
+      <c r="A2" s="5">
         <v>140</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="6">
         <v>45239.815914351901</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="6">
         <v>45239.819618055597</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="5">
         <v>2</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="5">
         <v>1</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="5">
         <v>1</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T2" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
-      <c r="A3">
+    <row r="3" spans="1:20" ht="15" customHeight="1">
+      <c r="A3" s="5">
         <v>175</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="6">
         <v>45239.816006944398</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="6">
         <v>45239.820381944402</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="5">
         <v>2</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="5">
         <v>1</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="5">
         <v>1</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="Q3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="T3" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
-      <c r="A4">
+    <row r="4" spans="1:20" ht="15" customHeight="1">
+      <c r="A4" s="5">
         <v>36</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="6">
         <v>45239.815949074102</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="6">
         <v>45239.818530092598</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="5">
         <v>2</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="5">
         <v>1</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="5">
         <v>1</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="Q4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="T4" s="3" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>